<commit_message>
Update ax new -- 17-05-2014
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 16.xlsx
+++ b/Fix/fix cur. 16.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>amt</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>24106000067272</t>
-  </si>
-  <si>
-    <t>912040060109592</t>
   </si>
   <si>
     <t>12+1</t>
@@ -254,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -402,6 +399,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -777,7 +777,7 @@
   <dimension ref="A1:U107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1013,97 +1013,97 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:21" s="51" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A7" s="47">
-        <v>5</v>
-      </c>
-      <c r="B7" s="47">
-        <v>9.75</v>
-      </c>
-      <c r="C7" s="47">
-        <v>18</v>
-      </c>
-      <c r="D7" s="47" t="s">
+    <row r="7" spans="1:21" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A7" s="30">
+        <v>12.3</v>
+      </c>
+      <c r="B7" s="30">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="C7" s="30">
+        <v>3</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48">
-        <v>41223</v>
-      </c>
-      <c r="H7" s="48">
-        <v>41769</v>
-      </c>
-      <c r="I7" s="28">
-        <v>4030</v>
-      </c>
-      <c r="J7" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="50"/>
-    </row>
-    <row r="8" spans="1:21" s="33" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A8" s="30">
-        <v>12.3</v>
-      </c>
-      <c r="B8" s="30">
-        <v>10.050000000000001</v>
-      </c>
-      <c r="C8" s="30">
-        <v>3</v>
-      </c>
-      <c r="D8" s="30" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="34">
+        <v>41304</v>
+      </c>
+      <c r="H7" s="34">
+        <v>42399</v>
+      </c>
+      <c r="I7" s="35">
+        <v>10215</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="30"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+    </row>
+    <row r="8" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A8" s="9">
+        <v>6.15</v>
+      </c>
+      <c r="B8" s="9">
+        <v>9.5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="34">
-        <v>41304</v>
-      </c>
-      <c r="H8" s="34">
-        <v>42399</v>
-      </c>
-      <c r="I8" s="35">
-        <v>10215</v>
+      <c r="F8" s="9"/>
+      <c r="G8" s="27">
+        <v>41480</v>
+      </c>
+      <c r="H8" s="27">
+        <v>42210</v>
+      </c>
+      <c r="I8" s="43">
+        <v>4830</v>
       </c>
       <c r="J8" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
+        <v>32</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
     </row>
     <row r="9" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="9">
-        <v>6.15</v>
+        <v>4.25</v>
       </c>
       <c r="B9" s="9">
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
       <c r="C9" s="9">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>6</v>
@@ -1113,17 +1113,15 @@
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="27">
-        <v>41480</v>
+        <v>41776</v>
       </c>
       <c r="H9" s="27">
-        <v>42210</v>
-      </c>
-      <c r="I9" s="43">
-        <v>4830</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>33</v>
-      </c>
+        <v>42141</v>
+      </c>
+      <c r="I9" s="55">
+        <v>3400</v>
+      </c>
+      <c r="J9" s="31"/>
       <c r="K9" s="9"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
@@ -1144,15 +1142,15 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <f>SUM(A7:A9)</f>
-        <v>23.450000000000003</v>
+        <v>22.700000000000003</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="8"/>
       <c r="J10" s="3"/>
       <c r="K10" s="8">
-        <f>SUM(I7:I9)</f>
-        <v>19075</v>
+        <f>SUM(I7:I8)</f>
+        <v>15045</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1173,7 +1171,7 @@
         <v>9.25</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>6</v>
@@ -1206,45 +1204,45 @@
       <c r="T11" s="39"/>
       <c r="U11" s="39"/>
     </row>
-    <row r="12" spans="1:21" ht="12.75" customHeight="1">
-      <c r="A12" s="3">
+    <row r="12" spans="1:21" s="51" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A12" s="47">
         <v>2.1</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="47">
         <v>9.75</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="23">
+      <c r="F12" s="47"/>
+      <c r="G12" s="48">
         <v>41312</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="48">
         <v>41812</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="28">
         <v>1692</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
+      <c r="J12" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
     </row>
     <row r="13" spans="1:21" s="12" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="9">
@@ -1254,7 +1252,7 @@
         <v>9.6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>6</v>
@@ -1295,7 +1293,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>6</v>
@@ -1314,7 +1312,7 @@
         <v>10125</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="11"/>
@@ -1384,7 +1382,7 @@
         <v>3353</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="11"/>
@@ -1425,7 +1423,7 @@
         <v>1811</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="11"/>
@@ -1447,7 +1445,7 @@
         <v>9.43</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>6</v>
@@ -1466,7 +1464,7 @@
         <v>2248</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="11"/>
@@ -1488,7 +1486,7 @@
         <v>9.43</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>6</v>
@@ -1507,7 +1505,7 @@
         <v>9531</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11"/>
@@ -1529,7 +1527,7 @@
         <v>9.43</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>6</v>
@@ -1548,7 +1546,7 @@
         <v>2500</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="11"/>
@@ -1640,7 +1638,7 @@
         <v>9.75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -1659,7 +1657,7 @@
         <v>3169</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="4"/>
@@ -1700,7 +1698,7 @@
         <v>2803</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
@@ -1741,7 +1739,7 @@
         <v>4672</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" s="3"/>
       <c r="L25" s="4"/>
@@ -1782,7 +1780,7 @@
         <v>2559</v>
       </c>
       <c r="J26" s="44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K26" s="41"/>
       <c r="L26" s="45"/>
@@ -1823,7 +1821,7 @@
         <v>3656</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="4"/>
@@ -1858,14 +1856,14 @@
         <v>41650</v>
       </c>
       <c r="H28" s="5">
-        <v>41650</v>
+        <v>43476</v>
       </c>
       <c r="I28" s="25">
         <f>1125/3</f>
         <v>375</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="4"/>
@@ -1941,13 +1939,13 @@
       <c r="E31" s="3"/>
       <c r="F31" s="1">
         <f>SUM(F3:F29)</f>
-        <v>114.5</v>
+        <v>113.75</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="7"/>
       <c r="I31" s="21">
         <f>SUM(I3:I27)</f>
-        <v>90436.666666666672</v>
+        <v>89806.666666666672</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>3</v>
@@ -2048,7 +2046,7 @@
       <c r="H35" s="4"/>
       <c r="I35" s="22">
         <f>I31+I33</f>
-        <v>107772.66666666667</v>
+        <v>107142.66666666667</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="3"/>

</xml_diff>

<commit_message>
Update ax latest FD No.
</commit_message>
<xml_diff>
--- a/Fix/fix cur. 16.xlsx
+++ b/Fix/fix cur. 16.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
   <si>
     <t>amt</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>50300041454823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">914040017483807 </t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -403,6 +406,12 @@
     </xf>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,7 +786,7 @@
   <dimension ref="A1:U107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -791,7 +800,7 @@
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="56" customWidth="1"/>
     <col min="11" max="21" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1121,7 +1130,9 @@
       <c r="I9" s="55">
         <v>3400</v>
       </c>
-      <c r="J9" s="31"/>
+      <c r="J9" s="57" t="s">
+        <v>43</v>
+      </c>
       <c r="K9" s="9"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
@@ -2022,7 +2033,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="26"/>
-      <c r="J34" s="4"/>
+      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
@@ -2048,7 +2059,7 @@
         <f>I31+I33</f>
         <v>107142.66666666667</v>
       </c>
-      <c r="J35" s="4"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
@@ -2071,7 +2082,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2093,7 +2104,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
@@ -2116,7 +2127,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="8"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
@@ -2139,7 +2150,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -2162,7 +2173,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
@@ -2185,7 +2196,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="26"/>
       <c r="I41" s="26"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
@@ -2208,7 +2219,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
+      <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
@@ -2231,7 +2242,7 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
@@ -2254,7 +2265,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
@@ -2277,7 +2288,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
+      <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
@@ -2300,7 +2311,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
@@ -2323,7 +2334,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
+      <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
@@ -2346,7 +2357,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
+      <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
@@ -2369,7 +2380,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
+      <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
@@ -2392,7 +2403,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
+      <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
@@ -2415,7 +2426,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
+      <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
@@ -2438,7 +2449,7 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
+      <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
@@ -2461,7 +2472,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
+      <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
@@ -2484,7 +2495,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
+      <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
@@ -2507,7 +2518,7 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
+      <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
@@ -2530,7 +2541,7 @@
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
+      <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
@@ -2553,7 +2564,7 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
@@ -2576,7 +2587,7 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
+      <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
@@ -2599,7 +2610,7 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
+      <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
@@ -2622,7 +2633,7 @@
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
+      <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
@@ -2645,7 +2656,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
+      <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -2668,7 +2679,7 @@
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
+      <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
@@ -2691,7 +2702,7 @@
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
+      <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
@@ -2714,7 +2725,7 @@
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
+      <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
@@ -2737,7 +2748,7 @@
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
+      <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
@@ -2760,7 +2771,7 @@
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
+      <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
@@ -2783,7 +2794,7 @@
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
+      <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
@@ -2806,7 +2817,7 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
+      <c r="J68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
@@ -2829,7 +2840,7 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
+      <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
@@ -2852,7 +2863,7 @@
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
+      <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
@@ -2875,7 +2886,7 @@
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
+      <c r="J71" s="3"/>
       <c r="K71" s="3"/>
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
@@ -2898,7 +2909,7 @@
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
+      <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
@@ -2921,7 +2932,7 @@
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
+      <c r="J73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
@@ -2944,7 +2955,7 @@
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
+      <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
@@ -2967,7 +2978,7 @@
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
+      <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
@@ -2990,7 +3001,7 @@
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
+      <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -3013,7 +3024,7 @@
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
+      <c r="J77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="4"/>
       <c r="M77" s="4"/>
@@ -3036,7 +3047,7 @@
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
+      <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="4"/>
       <c r="M78" s="4"/>
@@ -3059,7 +3070,7 @@
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
+      <c r="J79" s="3"/>
       <c r="K79" s="3"/>
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
@@ -3082,7 +3093,7 @@
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
+      <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
@@ -3105,7 +3116,7 @@
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
+      <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
@@ -3128,7 +3139,7 @@
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
+      <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
@@ -3151,7 +3162,7 @@
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
+      <c r="J83" s="3"/>
       <c r="K83" s="3"/>
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
@@ -3174,7 +3185,7 @@
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
+      <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
@@ -3197,7 +3208,7 @@
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
+      <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
@@ -3220,7 +3231,7 @@
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
+      <c r="J86" s="3"/>
       <c r="K86" s="3"/>
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
@@ -3243,7 +3254,7 @@
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
+      <c r="J87" s="3"/>
       <c r="K87" s="3"/>
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
@@ -3266,7 +3277,7 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
+      <c r="J88" s="3"/>
       <c r="K88" s="3"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
@@ -3289,7 +3300,7 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
-      <c r="J89" s="4"/>
+      <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
@@ -3312,7 +3323,7 @@
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
+      <c r="J90" s="3"/>
       <c r="K90" s="3"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
@@ -3335,7 +3346,7 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
+      <c r="J91" s="3"/>
       <c r="K91" s="3"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
@@ -3358,7 +3369,7 @@
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
+      <c r="J92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
@@ -3381,7 +3392,7 @@
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
+      <c r="J93" s="3"/>
       <c r="K93" s="3"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
@@ -3404,7 +3415,7 @@
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
-      <c r="J94" s="4"/>
+      <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
@@ -3427,7 +3438,7 @@
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
-      <c r="J95" s="4"/>
+      <c r="J95" s="3"/>
       <c r="K95" s="3"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
@@ -3450,7 +3461,7 @@
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
-      <c r="J96" s="4"/>
+      <c r="J96" s="3"/>
       <c r="K96" s="3"/>
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
@@ -3473,7 +3484,7 @@
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
+      <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
@@ -3496,7 +3507,7 @@
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
-      <c r="J98" s="4"/>
+      <c r="J98" s="3"/>
       <c r="K98" s="3"/>
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
@@ -3519,7 +3530,7 @@
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
+      <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
@@ -3542,7 +3553,7 @@
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
-      <c r="J100" s="4"/>
+      <c r="J100" s="3"/>
       <c r="K100" s="3"/>
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
@@ -3565,7 +3576,7 @@
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
-      <c r="J101" s="4"/>
+      <c r="J101" s="3"/>
       <c r="K101" s="3"/>
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
@@ -3588,7 +3599,7 @@
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
-      <c r="J102" s="4"/>
+      <c r="J102" s="3"/>
       <c r="K102" s="3"/>
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
@@ -3611,7 +3622,7 @@
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
+      <c r="J103" s="3"/>
       <c r="K103" s="3"/>
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
@@ -3634,7 +3645,7 @@
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
-      <c r="J104" s="4"/>
+      <c r="J104" s="3"/>
       <c r="K104" s="3"/>
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
@@ -3657,7 +3668,7 @@
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
-      <c r="J105" s="4"/>
+      <c r="J105" s="3"/>
       <c r="K105" s="3"/>
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
@@ -3680,7 +3691,7 @@
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
-      <c r="J106" s="4"/>
+      <c r="J106" s="3"/>
       <c r="K106" s="3"/>
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
@@ -3703,7 +3714,7 @@
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
-      <c r="J107" s="4"/>
+      <c r="J107" s="3"/>
       <c r="K107" s="3"/>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>

</xml_diff>